<commit_message>
Adding contribution details and expanding on the reflections
</commit_message>
<xml_diff>
--- a/Contribution Summary - Final.xlsx
+++ b/Contribution Summary - Final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8207bcd4c4ed8cf/Masters of Data Science/DSCI-D532/Final Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marfe\Desktop\Courses\Semester 2\Applied Database Technologies\Project\ADT-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{C7D7FA91-4FFA-45E7-A49C-59BBF9EC58AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{914936B8-EE08-4D1D-B925-9B7977DDDA61}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EDCC20-662A-4C25-A7A8-F1B77FDCB02A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{248FD177-A6C4-4547-84A7-5795F7ADDF04}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{248FD177-A6C4-4547-84A7-5795F7ADDF04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -129,6 +129,18 @@
   </si>
   <si>
     <t>Added screenshots, wrote and formatted text, added notes for presentation</t>
+  </si>
+  <si>
+    <t>Final formatting details and cohesion check</t>
+  </si>
+  <si>
+    <t>Created dashboard to see sales and profits given certain regions</t>
+  </si>
+  <si>
+    <t>Added screenshots and description of app functionality with the help of all team members</t>
+  </si>
+  <si>
+    <t>Description of team reflections on what we learned during this project and the most interesting parts</t>
   </si>
 </sst>
 </file>
@@ -529,18 +541,18 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="80" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,7 +566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -568,7 +580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -582,7 +594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -596,7 +608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -610,7 +622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -624,7 +636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -638,7 +650,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -652,7 +664,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -666,51 +678,63 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
       <c r="D10">
         <v>2.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
       </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
       <c r="D11">
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
       <c r="D12">
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
       </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
       <c r="D13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -721,7 +745,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -732,7 +756,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>

</xml_diff>